<commit_message>
Daily MPR update | 05-02-26
</commit_message>
<xml_diff>
--- a/MPR/Role wise/Software Developer/Feb'26/MPR-Feb'26.xlsx
+++ b/MPR/Role wise/Software Developer/Feb'26/MPR-Feb'26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Important\TH-PROJECT-NOTEBOOK\MPR\Role wise\Software Developer\Feb'26\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAEA8B6-E11D-40DF-8B2C-F1B6E130AFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D933697-BBC5-46A5-8727-2BD57D3A1C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>SR#</t>
   </si>
@@ -75,10 +75,16 @@
     <t>Working on Reporting Section: (1) Headers - Geographical, Departments, Schemes and PLD wise</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Working on Reporting Section: (1) Headers - Working on Scheme Code bug, Support bucket and Date filters.                (2) Body - Report table and Excel-Export Button</t>
+  </si>
+  <si>
+    <t>Switched to setup for Staging server provided by the Department for Hosting and security audit,                                  (1) Migration of Test DB, with the exact collation and schema as the real one.</t>
+  </si>
+  <si>
+    <t>Reporting Section of LDMS Pending, Validation setup and hardening of TMS pending.</t>
+  </si>
+  <si>
+    <t>Validation setup and hardening of TMS pending.</t>
   </si>
 </sst>
 </file>
@@ -499,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6806E486-C456-4888-BB52-4614915FD5B3}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +556,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -564,13 +570,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="5">
-        <v>46058</v>
+        <v>46059</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -591,7 +597,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -600,12 +606,37 @@
         <v>8</v>
       </c>
       <c r="E5" s="5">
-        <v>46058</v>
+        <v>46059</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>46065</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>